<commit_message>
Agrego campo superThemeTaxonomy al catálogo de ejemplo 1.
</commit_message>
<xml_diff>
--- a/samples/catalogs/example_catalog1.xlsx
+++ b/samples/catalogs/example_catalog1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="217">
   <si>
     <t>catalog_identifier</t>
   </si>
@@ -81,6 +81,9 @@
     <t>SPA</t>
   </si>
   <si>
+    <t>http://datos.gob.ar/superThemeTaxonomy.json</t>
+  </si>
+  <si>
     <t>Open Database License (ODbL) v1.0</t>
   </si>
   <si>
@@ -318,10 +321,10 @@
     <t>field_specialTypeDetail</t>
   </si>
   <si>
+    <t>field_specialType</t>
+  </si>
+  <si>
     <t>field_units</t>
-  </si>
-  <si>
-    <t>field_specialType</t>
   </si>
   <si>
     <t>indice_tiempo</t>
@@ -1076,14 +1079,17 @@
       <c r="H2" t="s">
         <v>19</v>
       </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1107,75 +1113,75 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Q1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -1187,51 +1193,51 @@
         <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
       </c>
       <c r="M2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N2" t="s">
         <v>19</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="S2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="T2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -1243,16 +1249,16 @@
         <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L3" t="s">
         <v>18</v>
@@ -1261,16 +1267,16 @@
         <v>19</v>
       </c>
       <c r="O3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="T3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1294,171 +1300,169 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="L1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Q1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" t="s"/>
+        <v>79</v>
+      </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M2" t="s">
         <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Q2" t="b">
         <v>0</v>
       </c>
       <c r="R2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" t="s"/>
+        <v>86</v>
+      </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M3" t="s">
         <v>18</v>
       </c>
       <c r="N3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="Q3" t="b">
         <v>0</v>
       </c>
       <c r="R3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M4" t="s">
         <v>18</v>
@@ -1485,768 +1489,768 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K2" t="s">
-        <v>106</v>
-      </c>
-      <c r="M2" t="s">
         <v>107</v>
+      </c>
+      <c r="L2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J3" t="s">
-        <v>113</v>
-      </c>
-      <c r="L3" t="s">
         <v>114</v>
+      </c>
+      <c r="M3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" t="s">
+        <v>120</v>
+      </c>
+      <c r="M4" t="s">
         <v>115</v>
-      </c>
-      <c r="F4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H4" t="s">
-        <v>117</v>
-      </c>
-      <c r="I4" t="s">
-        <v>118</v>
-      </c>
-      <c r="J4" t="s">
-        <v>119</v>
-      </c>
-      <c r="L4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J5" t="s">
-        <v>124</v>
-      </c>
-      <c r="L5" t="s">
-        <v>114</v>
+        <v>125</v>
+      </c>
+      <c r="M5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J6" t="s">
-        <v>129</v>
-      </c>
-      <c r="L6" t="s">
-        <v>114</v>
+        <v>130</v>
+      </c>
+      <c r="M6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J7" t="s">
-        <v>134</v>
-      </c>
-      <c r="L7" t="s">
-        <v>114</v>
+        <v>135</v>
+      </c>
+      <c r="M7" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J8" t="s">
-        <v>139</v>
-      </c>
-      <c r="L8" t="s">
-        <v>114</v>
+        <v>140</v>
+      </c>
+      <c r="M8" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K9" t="s">
-        <v>48</v>
-      </c>
-      <c r="M9" t="s">
-        <v>107</v>
+        <v>49</v>
+      </c>
+      <c r="L9" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J10" t="s">
-        <v>146</v>
-      </c>
-      <c r="L10" t="s">
-        <v>114</v>
+        <v>147</v>
+      </c>
+      <c r="M10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" t="s">
+        <v>148</v>
+      </c>
+      <c r="H11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I11" t="s">
+        <v>150</v>
+      </c>
+      <c r="J11" t="s">
+        <v>151</v>
+      </c>
+      <c r="M11" t="s">
         <v>115</v>
-      </c>
-      <c r="F11" t="s">
-        <v>109</v>
-      </c>
-      <c r="G11" t="s">
-        <v>147</v>
-      </c>
-      <c r="H11" t="s">
-        <v>148</v>
-      </c>
-      <c r="I11" t="s">
-        <v>149</v>
-      </c>
-      <c r="J11" t="s">
-        <v>150</v>
-      </c>
-      <c r="L11" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J12" t="s">
-        <v>154</v>
-      </c>
-      <c r="L12" t="s">
-        <v>114</v>
+        <v>155</v>
+      </c>
+      <c r="M12" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I13" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J13" t="s">
-        <v>158</v>
-      </c>
-      <c r="L13" t="s">
-        <v>114</v>
+        <v>159</v>
+      </c>
+      <c r="M13" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H14" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I14" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J14" t="s">
-        <v>162</v>
-      </c>
-      <c r="L14" t="s">
-        <v>114</v>
+        <v>163</v>
+      </c>
+      <c r="M14" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F15" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J15" t="s">
-        <v>166</v>
-      </c>
-      <c r="L15" t="s">
-        <v>114</v>
+        <v>167</v>
+      </c>
+      <c r="M15" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L16" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="M16" t="s">
-        <v>107</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E17" t="s">
+        <v>170</v>
+      </c>
+      <c r="F17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" t="s">
+        <v>171</v>
+      </c>
+      <c r="I17" t="s">
+        <v>172</v>
+      </c>
+      <c r="M17" t="s">
         <v>169</v>
-      </c>
-      <c r="F17" t="s">
-        <v>109</v>
-      </c>
-      <c r="G17" t="s">
-        <v>170</v>
-      </c>
-      <c r="I17" t="s">
-        <v>171</v>
-      </c>
-      <c r="L17" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E18" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I18" t="s">
-        <v>174</v>
-      </c>
-      <c r="L18" t="s">
-        <v>168</v>
+        <v>175</v>
+      </c>
+      <c r="M18" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I19" t="s">
-        <v>177</v>
-      </c>
-      <c r="L19" t="s">
-        <v>168</v>
+        <v>178</v>
+      </c>
+      <c r="M19" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I20" t="s">
-        <v>180</v>
-      </c>
-      <c r="L20" t="s">
-        <v>168</v>
+        <v>181</v>
+      </c>
+      <c r="M20" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G21" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I21" t="s">
-        <v>183</v>
-      </c>
-      <c r="L21" t="s">
-        <v>168</v>
+        <v>184</v>
+      </c>
+      <c r="M21" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F22" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G22" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I22" t="s">
-        <v>186</v>
-      </c>
-      <c r="L22" t="s">
-        <v>168</v>
+        <v>187</v>
+      </c>
+      <c r="M22" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G23" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I23" t="s">
-        <v>189</v>
-      </c>
-      <c r="L23" t="s">
-        <v>168</v>
+        <v>190</v>
+      </c>
+      <c r="M23" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2270,101 +2274,101 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C5" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Elimino algunas columnas innecesarias y ajusto los anchos para facilitar la lectura.
</commit_message>
<xml_diff>
--- a/samples/catalogs/example_catalog1.xlsx
+++ b/samples/catalogs/example_catalog1.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15620"/>
   </bookViews>
   <sheets>
-    <sheet name="catalog" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="dataset" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="distribution" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="field" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="theme" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="catalog" sheetId="1" r:id="rId1"/>
+    <sheet name="dataset" sheetId="2" r:id="rId2"/>
+    <sheet name="distribution" sheetId="3" r:id="rId3"/>
+    <sheet name="field" sheetId="4" r:id="rId4"/>
+    <sheet name="theme" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="214">
   <si>
     <t>catalog_identifier</t>
   </si>
@@ -147,9 +151,6 @@
     <t>dataset_source</t>
   </si>
   <si>
-    <t>dataset_accessLevel</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -183,9 +184,6 @@
     <t>Instituto Nacional de Estadística y Censos (INDEC)</t>
   </si>
   <si>
-    <t>ABIERTO</t>
-  </si>
-  <si>
     <t>200</t>
   </si>
   <si>
@@ -244,9 +242,6 @@
   </si>
   <si>
     <t>distribution_scrapingFileURL</t>
-  </si>
-  <si>
-    <t>distribution_draft</t>
   </si>
   <si>
     <t>distribution_scrapingFileSheet</t>
@@ -675,20 +670,35 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -703,16 +713,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+  <cellStyles count="11">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -1000,492 +1037,535 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" ht="28">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:T3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="42" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.83203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2" spans="1:19" s="2" customFormat="1" ht="42">
+      <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="s">
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="2" customFormat="1" ht="28">
+      <c r="A3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="J3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="L3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="N3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P2" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="P3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="S3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" t="s">
-        <v>59</v>
-      </c>
-      <c r="S3" t="s">
-        <v>60</v>
-      </c>
-      <c r="T3" t="s">
-        <v>54</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:R4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="51.33203125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="39" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="16.83203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="27.83203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="39" style="2" customWidth="1"/>
+    <col min="17" max="17" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17" ht="28">
+      <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="P1" t="s">
+    </row>
+    <row r="2" spans="1:17" ht="42">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="D2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="R1" t="s">
+      <c r="E2" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="42">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I2" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" t="s">
+    </row>
+    <row r="4" spans="1:17" ht="42">
+      <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I4" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" t="s">
-        <v>18</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -1495,139 +1575,139 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" t="s">
         <v>93</v>
-      </c>
-      <c r="F1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J1" t="s">
-        <v>98</v>
-      </c>
-      <c r="K1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L1" t="s">
-        <v>100</v>
-      </c>
-      <c r="M1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
         <v>102</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" t="s">
         <v>103</v>
       </c>
-      <c r="H2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J2" t="s">
-        <v>106</v>
-      </c>
-      <c r="K2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L2" t="s">
-        <v>108</v>
+      <c r="M2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" t="s">
+        <v>111</v>
+      </c>
+      <c r="M3" t="s">
         <v>109</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H3" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" t="s">
-        <v>113</v>
-      </c>
-      <c r="J3" t="s">
-        <v>114</v>
-      </c>
-      <c r="M3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" t="s">
         <v>116</v>
       </c>
-      <c r="F4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L4" t="s">
         <v>117</v>
-      </c>
-      <c r="H4" t="s">
-        <v>118</v>
-      </c>
-      <c r="I4" t="s">
-        <v>119</v>
-      </c>
-      <c r="J4" t="s">
-        <v>120</v>
       </c>
       <c r="M4" t="s">
         <v>115</v>
@@ -1635,743 +1715,755 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" t="s">
         <v>121</v>
       </c>
-      <c r="F5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
+        <v>112</v>
+      </c>
+      <c r="L5" t="s">
         <v>122</v>
       </c>
-      <c r="H5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I5" t="s">
-        <v>124</v>
-      </c>
-      <c r="J5" t="s">
-        <v>125</v>
-      </c>
       <c r="M5" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" t="s">
         <v>126</v>
       </c>
-      <c r="F6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L6" t="s">
         <v>127</v>
       </c>
-      <c r="H6" t="s">
-        <v>128</v>
-      </c>
-      <c r="I6" t="s">
-        <v>129</v>
-      </c>
-      <c r="J6" t="s">
-        <v>130</v>
-      </c>
       <c r="M6" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" t="s">
         <v>131</v>
       </c>
-      <c r="F7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L7" t="s">
         <v>132</v>
       </c>
-      <c r="H7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I7" t="s">
-        <v>134</v>
-      </c>
-      <c r="J7" t="s">
-        <v>135</v>
-      </c>
       <c r="M7" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H8" t="s">
         <v>136</v>
       </c>
-      <c r="F8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
+        <v>112</v>
+      </c>
+      <c r="L8" t="s">
         <v>137</v>
       </c>
-      <c r="H8" t="s">
-        <v>138</v>
-      </c>
-      <c r="I8" t="s">
-        <v>139</v>
-      </c>
-      <c r="J8" t="s">
-        <v>140</v>
-      </c>
       <c r="M8" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H9" t="s">
-        <v>141</v>
-      </c>
-      <c r="I9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J9" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="K9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L9" t="s">
-        <v>108</v>
+        <v>140</v>
+      </c>
+      <c r="M9" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" t="s">
+        <v>112</v>
+      </c>
+      <c r="L10" t="s">
         <v>144</v>
       </c>
-      <c r="H10" t="s">
-        <v>145</v>
-      </c>
-      <c r="I10" t="s">
-        <v>146</v>
-      </c>
-      <c r="J10" t="s">
-        <v>147</v>
-      </c>
       <c r="M10" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
-        <v>44</v>
-      </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L11" t="s">
         <v>148</v>
       </c>
-      <c r="H11" t="s">
-        <v>149</v>
-      </c>
-      <c r="I11" t="s">
-        <v>150</v>
-      </c>
-      <c r="J11" t="s">
-        <v>151</v>
-      </c>
       <c r="M11" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
         <v>43</v>
       </c>
-      <c r="B12" t="s">
-        <v>44</v>
-      </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G12" t="s">
+        <v>149</v>
+      </c>
+      <c r="H12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I12" t="s">
+        <v>112</v>
+      </c>
+      <c r="L12" t="s">
         <v>152</v>
       </c>
-      <c r="H12" t="s">
-        <v>153</v>
-      </c>
-      <c r="I12" t="s">
-        <v>154</v>
-      </c>
-      <c r="J12" t="s">
-        <v>155</v>
-      </c>
       <c r="M12" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G13" t="s">
+        <v>153</v>
+      </c>
+      <c r="H13" t="s">
+        <v>155</v>
+      </c>
+      <c r="I13" t="s">
+        <v>112</v>
+      </c>
+      <c r="L13" t="s">
         <v>156</v>
       </c>
-      <c r="H13" t="s">
-        <v>157</v>
-      </c>
-      <c r="I13" t="s">
-        <v>158</v>
-      </c>
-      <c r="J13" t="s">
-        <v>159</v>
-      </c>
       <c r="M13" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G14" t="s">
+        <v>157</v>
+      </c>
+      <c r="H14" t="s">
+        <v>159</v>
+      </c>
+      <c r="I14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L14" t="s">
         <v>160</v>
       </c>
-      <c r="H14" t="s">
-        <v>161</v>
-      </c>
-      <c r="I14" t="s">
-        <v>162</v>
-      </c>
-      <c r="J14" t="s">
-        <v>163</v>
-      </c>
       <c r="M14" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I15" t="s">
+        <v>112</v>
+      </c>
+      <c r="L15" t="s">
         <v>164</v>
       </c>
-      <c r="H15" t="s">
-        <v>165</v>
-      </c>
-      <c r="I15" t="s">
-        <v>166</v>
-      </c>
-      <c r="J15" t="s">
-        <v>167</v>
-      </c>
       <c r="M15" t="s">
-        <v>115</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>100</v>
+      </c>
+      <c r="H16" t="s">
+        <v>165</v>
       </c>
       <c r="I16" t="s">
+        <v>166</v>
+      </c>
+      <c r="J16" t="s">
+        <v>105</v>
+      </c>
+      <c r="K16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" t="s">
         <v>168</v>
       </c>
-      <c r="K16" t="s">
-        <v>49</v>
-      </c>
-      <c r="L16" t="s">
-        <v>108</v>
-      </c>
-      <c r="M16" t="s">
+      <c r="H17" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="I17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" t="s">
         <v>170</v>
       </c>
-      <c r="F17" t="s">
-        <v>110</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="F18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" t="s">
         <v>171</v>
       </c>
-      <c r="I17" t="s">
+      <c r="H18" t="s">
         <v>172</v>
       </c>
-      <c r="M17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="I18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
         <v>173</v>
       </c>
-      <c r="F18" t="s">
-        <v>110</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="F19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" t="s">
         <v>174</v>
       </c>
-      <c r="I18" t="s">
+      <c r="H19" t="s">
         <v>175</v>
       </c>
-      <c r="M18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="I19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" t="s">
         <v>176</v>
       </c>
-      <c r="F19" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="F20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" t="s">
         <v>177</v>
       </c>
-      <c r="I19" t="s">
+      <c r="H20" t="s">
         <v>178</v>
       </c>
-      <c r="M19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="I20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" t="s">
         <v>179</v>
       </c>
-      <c r="F20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="F21" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" t="s">
         <v>180</v>
       </c>
-      <c r="I20" t="s">
+      <c r="H21" t="s">
         <v>181</v>
       </c>
-      <c r="M20" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="I21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" t="s">
         <v>182</v>
       </c>
-      <c r="F21" t="s">
-        <v>110</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="F22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" t="s">
         <v>183</v>
       </c>
-      <c r="I21" t="s">
+      <c r="H22" t="s">
         <v>184</v>
       </c>
-      <c r="M21" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="I22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" t="s">
         <v>185</v>
       </c>
-      <c r="F22" t="s">
-        <v>110</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" t="s">
         <v>186</v>
       </c>
-      <c r="I22" t="s">
+      <c r="H23" t="s">
         <v>187</v>
       </c>
-      <c r="M22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F23" t="s">
-        <v>110</v>
-      </c>
-      <c r="G23" t="s">
-        <v>189</v>
-      </c>
       <c r="I23" t="s">
-        <v>190</v>
-      </c>
-      <c r="M23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>